<commit_message>
RF classify (read data header bug)
</commit_message>
<xml_diff>
--- a/Data/original_data/160608_Phase.xlsx
+++ b/Data/original_data/160608_Phase.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moliang\Documents\MATLAB\AIM2_AP\Phase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="3640" windowWidth="16500" windowHeight="8680" tabRatio="500"/>
+    <workbookView xWindow="7935" yWindow="3645" windowWidth="16500" windowHeight="8685" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="160608_Phase" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>start time</t>
   </si>
@@ -55,9 +60,6 @@
   </si>
   <si>
     <t>Pt departure</t>
-  </si>
-  <si>
-    <t>Video start time:</t>
   </si>
 </sst>
 </file>
@@ -65,9 +67,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,13 +89,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,10 +118,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -137,6 +131,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -462,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,32 +491,12 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>H2-B$9</f>
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <f>I2-B$9</f>
         <v>4.8263888888888662E-3</v>
       </c>
       <c r="C2" t="s">
@@ -526,29 +508,12 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.82990740740740743</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.83473379629629629</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A7" si="0">H3-B$9</f>
         <v>4.8263888888888662E-3</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B7" si="1">I3-B$9</f>
         <v>5.2777777777777146E-3</v>
       </c>
       <c r="C3" t="s">
@@ -560,30 +525,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
-        <f>I2</f>
-        <v>0.83473379629629629</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.83518518518518514</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" si="0"/>
         <v>5.2893518518518645E-3</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="1"/>
         <v>7.222222222222241E-3</v>
       </c>
       <c r="C4" t="s">
@@ -595,29 +542,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.83519675925925929</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.83712962962962967</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
         <v>7.222222222222241E-3</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="1"/>
         <v>9.9652777777777812E-3</v>
       </c>
       <c r="C5" t="s">
@@ -629,30 +559,12 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <f>I4</f>
-        <v>0.83712962962962967</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.83987268518518521</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
         <v>9.9652777777777812E-3</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="1"/>
         <v>1.7951388888888919E-2</v>
       </c>
       <c r="C6" t="s">
@@ -664,30 +576,12 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="H6" s="1">
-        <f>I5</f>
-        <v>0.83987268518518521</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.84785879629629635</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
         <v>1.7951388888888919E-2</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="1"/>
         <v>1.7962962962962958E-2</v>
       </c>
       <c r="C7" t="s">
@@ -698,41 +592,11 @@
       </c>
       <c r="E7">
         <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <f>I6</f>
-        <v>0.84785879629629635</v>
-      </c>
-      <c r="I7" s="1">
-        <f>H7+B$11</f>
-        <v>0.84787037037037039</v>
-      </c>
-      <c r="J7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.82990740740740743</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="B11" s="2">
-        <v>1.1574074074074073E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>